<commit_message>
CIDC-1410 add fix for clinical data participant counting
</commit_message>
<xml_diff>
--- a/tests/data/clinical_test_file.1.xlsx
+++ b/tests/data/clinical_test_file.1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10323"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jlindsay/Code/CIDC/cidc-schemas/tests/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu-20.04\home\jamesp\cidc-schemas\tests\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95596D43-C699-D641-AE85-E362D3356A77}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACC245FA-3BE7-4F05-82AA-1A7C85D65143}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2800" yWindow="2440" windowWidth="24180" windowHeight="11600" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="33135" yWindow="-9915" windowWidth="15375" windowHeight="7875" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
@@ -528,121 +528,121 @@
   <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="G5" sqref="G2:G5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.5" defaultRowHeight="14"/>
+  <sheetFormatPr defaultColWidth="10.5" defaultRowHeight="14.25"/>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1" ht="28" customHeight="1">
+    <row r="1" spans="1:7" s="1" customFormat="1" ht="27.95" customHeight="1">
       <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>6</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:7">
       <c r="A2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G2" t="s">
         <v>7</v>
-      </c>
-      <c r="B2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G2" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="B3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D3" t="s">
         <v>11</v>
       </c>
       <c r="E3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G3" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:7">
+      <c r="A4" t="s">
+        <v>10</v>
+      </c>
       <c r="B4" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D4" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="E4" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="F4" t="s">
-        <v>10</v>
-      </c>
-      <c r="G4" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:7">
       <c r="A5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F5" t="s">
+        <v>10</v>
+      </c>
+      <c r="G5" t="s">
         <v>9</v>
-      </c>
-      <c r="B5" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5" t="s">
-        <v>12</v>
-      </c>
-      <c r="D5" t="s">
-        <v>11</v>
-      </c>
-      <c r="E5" t="s">
-        <v>13</v>
-      </c>
-      <c r="F5" t="s">
-        <v>10</v>
-      </c>
-      <c r="G5" t="s">
-        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -659,7 +659,7 @@
       <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25"/>
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" t="s">

</xml_diff>